<commit_message>
update to user stories
</commit_message>
<xml_diff>
--- a/User Stories/User Stories Total.xlsx
+++ b/User Stories/User Stories Total.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin mills\Desktop\Year3_SoftwareEngineering3_Assignment\User_Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin mills\Desktop\Year3_SoftwareEngineering3_Assignment\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E22CB41-F34E-4A32-BE2F-219EED79882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A91A1D7-B7B6-49B9-B611-57D95187CEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8AD5C12C-F69F-41CA-A49A-35D721082458}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{8AD5C12C-F69F-41CA-A49A-35D721082458}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="178">
   <si>
     <t>As a NewsAgent</t>
   </si>
@@ -86,15 +86,6 @@
     <t>Verify Valid Publication Id</t>
   </si>
   <si>
-    <t>Verify Valid Publication Price</t>
-  </si>
-  <si>
-    <t>Verify Valid shcedule</t>
-  </si>
-  <si>
-    <t>Verify Valid Name</t>
-  </si>
-  <si>
     <t>I want to read Publication Information</t>
   </si>
   <si>
@@ -107,36 +98,12 @@
     <t>so that I can change the Publication details accordingly</t>
   </si>
   <si>
-    <t>Verify info succesfully changed</t>
-  </si>
-  <si>
     <t>Verify Valid Customer Order returned</t>
   </si>
   <si>
     <t>Verify absence state returned</t>
   </si>
   <si>
-    <t>verify other customer information remains unchanged</t>
-  </si>
-  <si>
-    <t>Verify Valid Publication Id returned</t>
-  </si>
-  <si>
-    <t>Verify Valid Publication Price returned</t>
-  </si>
-  <si>
-    <t>Verify Valid shcedule returned</t>
-  </si>
-  <si>
-    <t>Verify Valid Name returned</t>
-  </si>
-  <si>
-    <t>verify other publications information remains unchanged</t>
-  </si>
-  <si>
-    <t>verify info succesfully deleted</t>
-  </si>
-  <si>
     <t>I want to create a new order</t>
   </si>
   <si>
@@ -215,27 +182,6 @@
     <t xml:space="preserve">so that I can remove old invoice </t>
   </si>
   <si>
-    <t>Verify Valid bill Id</t>
-  </si>
-  <si>
-    <t>Verify Valid customer id</t>
-  </si>
-  <si>
-    <t>Verify Valid publications delivered</t>
-  </si>
-  <si>
-    <t>Verify total amount due</t>
-  </si>
-  <si>
-    <t>Verify Valid delivery Id</t>
-  </si>
-  <si>
-    <t>Verify Valid delivery date</t>
-  </si>
-  <si>
-    <t>Verify Valid list of publications delivered</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -461,28 +407,169 @@
     <t>verify customer details are displayed neatly</t>
   </si>
   <si>
-    <t>Verify Customer Phone Number is changed</t>
-  </si>
-  <si>
-    <t>Verify Address is changed from prevous to new address</t>
-  </si>
-  <si>
     <t>Verify customer details are all succesfully changed</t>
   </si>
   <si>
-    <t xml:space="preserve">Verfy customer name is changed </t>
-  </si>
-  <si>
     <t>verify customer is removed from the database</t>
   </si>
   <si>
-    <t>custmomer id</t>
-  </si>
-  <si>
-    <t>verfy valid publication type</t>
-  </si>
-  <si>
-    <t>customer order</t>
+    <t>Verify that no other customer details are affected.</t>
+  </si>
+  <si>
+    <t>Verify that the Publication ID is a valid integer.</t>
+  </si>
+  <si>
+    <t>Verify that the Publication Name contains only valid characters.</t>
+  </si>
+  <si>
+    <t>Verify that the Publication Price is a valid decimal number.</t>
+  </si>
+  <si>
+    <t>Verify that the publication type is correctly set.</t>
+  </si>
+  <si>
+    <t>Verify that a valid delivery frequency (daily, weekly)</t>
+  </si>
+  <si>
+    <t>Verify that the Publication Price is correctly displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the publication’s delivery schedule is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that publication type and other details are displayed.</t>
+  </si>
+  <si>
+    <t>Verify Publication Id is displayed</t>
+  </si>
+  <si>
+    <t>Verify that the Publication Price is updated to a valid decimal number.</t>
+  </si>
+  <si>
+    <t>Verify that the delivery schedule is successfully updated.</t>
+  </si>
+  <si>
+    <t>Verify that the publication type is correctly updated.</t>
+  </si>
+  <si>
+    <t>Verify publication details are succesfully changed</t>
+  </si>
+  <si>
+    <t>Verify that the Publication is successfully deleted from the system.</t>
+  </si>
+  <si>
+    <t>Verify that no other publications or orders are affected.</t>
+  </si>
+  <si>
+    <t>Verify that the Order ID is a valid integer.</t>
+  </si>
+  <si>
+    <t>Verify that a valid Customer ID is provided.</t>
+  </si>
+  <si>
+    <t>Verify that the order total price is correctly calculated based on the publication prices.</t>
+  </si>
+  <si>
+    <t>Verify that the order is successfully saved in the database.</t>
+  </si>
+  <si>
+    <t>Verify that the Customer ID associated with the order is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications ordered is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the total order price is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the order status (delivered, pending, etc.) is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications in the order can be successfully updated.</t>
+  </si>
+  <si>
+    <t>Verify that the total price is recalculated correctly based on any updates.</t>
+  </si>
+  <si>
+    <t>Verify that the customer and order details are successfully updated in the system.</t>
+  </si>
+  <si>
+    <t>Verify order details are succesfully changed</t>
+  </si>
+  <si>
+    <t>Verify that the order is successfully deleted from the system.</t>
+  </si>
+  <si>
+    <t>Verify that no related customer or publication details are affected.</t>
+  </si>
+  <si>
+    <t>Verify that the Delivery Docket ID is a valid integer.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications delivered is correct.</t>
+  </si>
+  <si>
+    <t>Verify that the delivery date and time are valid.</t>
+  </si>
+  <si>
+    <t>Verify that the order ID is a valid integer.</t>
+  </si>
+  <si>
+    <t>Verify that a valid Customer ID is a valid integer</t>
+  </si>
+  <si>
+    <t>Verify that a valid delivery ID is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the customer ID is correctly shown.</t>
+  </si>
+  <si>
+    <t>Verify that the delivery date is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications delivered is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the delivery date is successfully updated.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications delivered is successfully updated.</t>
+  </si>
+  <si>
+    <t>Verify that the delivery docket is successfully deleted from the system.</t>
+  </si>
+  <si>
+    <t>Verify that no other customer or publication details are affected.</t>
+  </si>
+  <si>
+    <t>Verify that the invoice ID is valid.</t>
+  </si>
+  <si>
+    <t>Verify that the customer ID is valid.</t>
+  </si>
+  <si>
+    <t>Verify the total amount due is correctly calculated.</t>
+  </si>
+  <si>
+    <t>Verify that the order ID is valid.</t>
+  </si>
+  <si>
+    <t>Verify that the customer ID is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the list of publications delivered is shown.</t>
+  </si>
+  <si>
+    <t>Verify that the total amount due is displayed.</t>
+  </si>
+  <si>
+    <t>Verify that the order ID is displayed</t>
+  </si>
+  <si>
+    <t>Verify that the total amount due is successfully recalculated.</t>
+  </si>
+  <si>
+    <t>Verify that the invoice is successfully deleted from the system.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,6 +686,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -666,7 +759,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -697,9 +790,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -738,6 +828,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -953,8 +1055,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56C535F4-5C97-4BC8-993C-585DE7AB2A76}" name="Table1" displayName="Table1" ref="A118:C163" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" headerRowCellStyle="Heading 3">
-  <autoFilter ref="A118:C163" xr:uid="{56C535F4-5C97-4BC8-993C-585DE7AB2A76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56C535F4-5C97-4BC8-993C-585DE7AB2A76}" name="Table1" displayName="Table1" ref="A121:C166" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" headerRowCellStyle="Heading 3">
+  <autoFilter ref="A121:C166" xr:uid="{56C535F4-5C97-4BC8-993C-585DE7AB2A76}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FF5C2DBF-008D-4B8A-A3AF-D6FC58C99BF9}" name="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{61083DAD-75E6-40E0-8189-920F1443B7F6}" name="Daily Delivery List for Delivery Person" dataDxfId="1"/>
@@ -1281,17 +1383,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCF095A-A1DB-48F1-AFFA-C8095C4C1526}">
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1311,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,10 +1422,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,27 +1434,27 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1375,10 +1477,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1387,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,14 +1501,14 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -1416,7 +1518,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>6</v>
@@ -1434,8 +1536,8 @@
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>141</v>
+      <c r="C15" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,25 +1545,19 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>142</v>
-      </c>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>144</v>
-      </c>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1476,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1485,7 +1581,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1526,21 +1622,21 @@
         <v>14</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,32 +1652,32 @@
         <v>0</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,40 +1692,40 @@
       <c r="B36" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
-        <v>18</v>
+      <c r="C39" s="24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,47 +1741,39 @@
         <v>0</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="C47" s="4"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
@@ -1695,29 +1783,33 @@
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
@@ -1725,42 +1817,50 @@
       <c r="C53" s="10"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
+      <c r="A54" s="25">
         <v>10</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="10"/>
+      <c r="C54" s="25" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="10"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="10"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
@@ -1769,26 +1869,34 @@
       <c r="B60" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="10"/>
+      <c r="C60" s="27" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
+      <c r="C63" s="10" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
@@ -1801,37 +1909,41 @@
       <c r="C65" s="10"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="10">
+      <c r="A66" s="25">
         <v>12</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" s="25" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="10"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" s="10"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" s="25"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
@@ -1841,79 +1953,81 @@
         <v>0</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
-        <v>65</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
+      <c r="C76" s="6" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="6">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
         <v>14</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C78" s="6" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
+      <c r="B80" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C80" s="6" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
@@ -1921,40 +2035,36 @@
       <c r="C82" s="6"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="6">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
         <v>15</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B84" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="C84" s="6" t="s">
-        <v>60</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="B86" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C86" s="6"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
@@ -1967,603 +2077,610 @@
       <c r="C88" s="6"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="6">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
         <v>16</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B90" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="C90" s="6" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
-      <c r="B91" s="7" t="s">
-        <v>50</v>
+      <c r="B91" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="B92" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" s="6"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="8">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="8">
         <v>17</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B96" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C95" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="8"/>
-      <c r="B96" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="C96" s="8" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
+      <c r="B99" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
-        <v>18</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
       <c r="C100" s="8" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="8"/>
-      <c r="B101" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="8"/>
+      <c r="A102" s="8">
+        <v>18</v>
+      </c>
       <c r="B102" s="8" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="8"/>
-      <c r="B103" s="8"/>
+      <c r="B103" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="C103" s="8" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
+      <c r="C104" s="8" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
+      <c r="B105" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="8">
-        <v>19</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
       <c r="C106" s="8" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
-      <c r="B107" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="8"/>
-      <c r="B108" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
+      <c r="A109" s="8">
+        <v>19</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C109" s="8" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
+      <c r="B110" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
+      <c r="B111" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
-        <v>20</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="8"/>
-      <c r="B113" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="8"/>
-      <c r="B114" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
+      <c r="A115" s="8">
+        <v>20</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="C115" s="8" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="12" t="s">
+      <c r="B116" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C117" s="8"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="12"/>
+      <c r="B122" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="12"/>
+      <c r="B123" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="12"/>
+      <c r="B124" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C124" s="12"/>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="12"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+    </row>
+    <row r="126" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="13">
+        <v>2</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="13"/>
+      <c r="B127" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="13"/>
+      <c r="B128" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C128" s="13"/>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+    </row>
+    <row r="130" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="15">
+        <v>3</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C130" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="15"/>
+      <c r="B131" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="15"/>
+      <c r="B132" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C132" s="15"/>
+    </row>
+    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="12"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="12"/>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="13">
+        <v>4</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="13"/>
+      <c r="B135" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="C135" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C118" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="13"/>
-      <c r="B119" s="13" t="s">
+    </row>
+    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="13"/>
+      <c r="B136" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="C136" s="13"/>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+    </row>
+    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>6</v>
+      </c>
+      <c r="B138" s="14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="13"/>
-      <c r="B120" s="13" t="s">
+      <c r="C138" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C120" s="13" t="s">
+    </row>
+    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A139" s="14"/>
+      <c r="B139" s="14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="13"/>
-      <c r="B121" s="13" t="s">
+      <c r="C139" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C121" s="13"/>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="13"/>
-      <c r="B122" s="13"/>
-      <c r="C122" s="13"/>
-    </row>
-    <row r="123" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="14">
-        <v>2</v>
-      </c>
-      <c r="B123" s="14" t="s">
+    </row>
+    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="14"/>
+      <c r="B140" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C123" s="14" t="s">
+      <c r="C140" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14" t="s">
+    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C124" s="14" t="s">
+    </row>
+    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>8</v>
+      </c>
+      <c r="B143" s="14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14" t="s">
+      <c r="C143" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C125" s="14"/>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="15"/>
-      <c r="B126" s="15"/>
-      <c r="C126" s="15"/>
-    </row>
-    <row r="127" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="16">
-        <v>3</v>
-      </c>
-      <c r="B127" s="17" t="s">
+    </row>
+    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A144" s="14"/>
+      <c r="B144" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C127" s="16" t="s">
+      <c r="C144" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="16"/>
-      <c r="B128" s="16" t="s">
+    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A145" s="14"/>
+      <c r="B145" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C128" s="16" t="s">
+      <c r="C145" s="14"/>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="14"/>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="12">
+        <v>9</v>
+      </c>
+      <c r="B147" s="17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="16"/>
-      <c r="B129" s="16" t="s">
+      <c r="C147" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C129" s="16"/>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="13"/>
-      <c r="B130" s="13"/>
-      <c r="C130" s="13"/>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="14">
-        <v>4</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C131" s="14" t="s">
+    </row>
+    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A148" s="12"/>
+      <c r="B148" s="17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14" t="s">
+      <c r="C148" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C132" s="14" t="s">
+    </row>
+    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A149" s="12"/>
+      <c r="B149" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14" t="s">
+      <c r="C149" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C133" s="14"/>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="15"/>
-      <c r="B134" s="15"/>
-      <c r="C134" s="15"/>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="15">
-        <v>6</v>
-      </c>
-      <c r="B135" s="15" t="s">
+    </row>
+    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="12"/>
+      <c r="B150" s="12"/>
+      <c r="C150" s="12"/>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>10</v>
+      </c>
+      <c r="B151" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C135" s="15" t="s">
+      <c r="C151" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="15"/>
-      <c r="B136" s="15" t="s">
+    <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A152" s="14"/>
+      <c r="B152" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C136" s="15" t="s">
+      <c r="C152" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="15"/>
-      <c r="B137" s="15" t="s">
+    <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="14"/>
+      <c r="B153" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C153" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="15"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="15" t="s">
+    <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="14"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="14"/>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="12">
+        <v>11</v>
+      </c>
+      <c r="B155" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C155" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="15"/>
-      <c r="B139" s="15"/>
-      <c r="C139" s="15"/>
-    </row>
-    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="15">
-        <v>8</v>
-      </c>
-      <c r="B140" s="15" t="s">
+    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="12"/>
+      <c r="B156" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="C156" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="15"/>
-      <c r="B141" s="15" t="s">
+    <row r="157" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="12"/>
+      <c r="B157" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C141" s="15" t="s">
+      <c r="C157" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="15"/>
-      <c r="B142" s="15" t="s">
+    <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>12</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C158" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C142" s="15"/>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="15"/>
-      <c r="B143" s="15"/>
-      <c r="C143" s="15"/>
-    </row>
-    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="13">
-        <v>9</v>
-      </c>
-      <c r="B144" s="18" t="s">
+    </row>
+    <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A159" s="14"/>
+      <c r="B159" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C144" s="18" t="s">
+      <c r="C159" s="14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="13"/>
-      <c r="B145" s="18" t="s">
+    <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A160" s="14"/>
+      <c r="B160" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C145" s="18" t="s">
+      <c r="C160" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="13"/>
-      <c r="B146" s="18" t="s">
+    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A161" s="18">
+        <v>5</v>
+      </c>
+      <c r="B161" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C146" s="18" t="s">
+      <c r="C161" s="19"/>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C162" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="13"/>
-      <c r="B147" s="13"/>
-      <c r="C147" s="13"/>
-    </row>
-    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="15">
-        <v>10</v>
-      </c>
-      <c r="B148" s="15" t="s">
+    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="C163" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="15"/>
-      <c r="B149" s="15" t="s">
+    <row r="164" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="20"/>
+      <c r="B164" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C149" s="15" t="s">
+      <c r="C164" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="15"/>
-      <c r="B150" s="15" t="s">
+    <row r="165" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="20"/>
+      <c r="B165" s="20"/>
+      <c r="C165" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C150" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="15"/>
-      <c r="B151" s="15"/>
-      <c r="C151" s="15"/>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="13">
-        <v>11</v>
-      </c>
-      <c r="B152" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C152" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="13"/>
-      <c r="B153" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C153" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="13"/>
-      <c r="B154" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C154" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="15">
-        <v>12</v>
-      </c>
-      <c r="B155" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C155" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="15"/>
-      <c r="B156" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C156" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="15"/>
-      <c r="B157" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C157" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="19">
-        <v>5</v>
-      </c>
-      <c r="B158" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C158" s="20"/>
-    </row>
-    <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="21"/>
-      <c r="B159" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C159" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="21"/>
-      <c r="B160" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C160" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="21"/>
-      <c r="B161" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C161" s="21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="21"/>
-      <c r="B162" s="21"/>
-      <c r="C162" s="21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="22"/>
-      <c r="B163" s="22"/>
-      <c r="C163" s="23"/>
+    </row>
+    <row r="166" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A166" s="21"/>
+      <c r="B166" s="21"/>
+      <c r="C166" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>